<commit_message>
Added the findings in excel sheet
</commit_message>
<xml_diff>
--- a/DataSamplerate.xlsx
+++ b/DataSamplerate.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ramakrishnan\FRDM_KL25Z\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="8595" windowHeight="8265"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="8592" windowHeight="8268" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Data Capture" sheetId="1" r:id="rId1"/>
+    <sheet name="Data plot" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>UART Baud rate</t>
   </si>
@@ -31,16 +36,34 @@
   </si>
   <si>
     <t>S.No</t>
+  </si>
+  <si>
+    <t>S. No.</t>
+  </si>
+  <si>
+    <t>fps</t>
+  </si>
+  <si>
+    <t>HTML data plot</t>
+  </si>
+  <si>
+    <t>Data Points in Plot can be plotted</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -61,7 +84,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -78,10 +101,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -91,6 +126,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -139,7 +177,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -174,7 +212,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -385,17 +423,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
         <v>2</v>
       </c>
@@ -403,83 +442,83 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>115200</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <f>B3/10</f>
         <v>11520</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <f>C3/D$1</f>
         <v>2304</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="5">
         <f>B3*2</f>
         <v>230400</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="5">
         <f t="shared" ref="C4:C6" si="0">B4/10</f>
         <v>23040</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="5">
         <f t="shared" ref="D4:D6" si="1">C4/D$1</f>
         <v>4608</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="5">
         <f>B3*5</f>
         <v>576000</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="5">
         <f t="shared" si="0"/>
         <v>57600</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="5">
         <f t="shared" si="1"/>
         <v>11520</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <f>B3*6</f>
         <v>691200</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <f t="shared" si="0"/>
         <v>69120</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <f t="shared" si="1"/>
         <v>13824</v>
       </c>
@@ -491,13 +530,84 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4">
+        <v>60000</v>
+      </c>
+      <c r="E3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>30</v>
+      </c>
+      <c r="C4" s="4">
+        <v>20000</v>
+      </c>
+      <c r="E4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>50</v>
+      </c>
+      <c r="C5" s="4">
+        <v>15000</v>
+      </c>
+      <c r="E5">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -507,7 +617,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>